<commit_message>
rerun for some data
</commit_message>
<xml_diff>
--- a/new_data/BS_continuous_hedge.xlsx
+++ b/new_data/BS_continuous_hedge.xlsx
@@ -380,1702 +380,1702 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>155.2942617751159</v>
+        <v>-91.16821566073217</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>1314.14161503916</v>
+        <v>-87.35346209422079</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>-79.47748643001232</v>
+        <v>273.0040457132265</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>704.0098249137454</v>
+        <v>405.786971084272</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>1173.775866012987</v>
+        <v>66.69207041387241</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>59.86554051974473</v>
+        <v>218.7993986964535</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-169.4233251564316</v>
+        <v>66.19247727388235</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>-416.6012622580241</v>
+        <v>674.5833712898993</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>315.5506930990034</v>
+        <v>-693.8897294255598</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>-323.1991515993893</v>
+        <v>-117.1617919057198</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>671.8174392792798</v>
+        <v>507.5938526504582</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>20848.27175490239</v>
+        <v>1306.832307327348</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>-19495.60165142112</v>
+        <v>-217.5515516225209</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>18765.65308897821</v>
+        <v>1018.700764820699</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>-15338.17707785995</v>
+        <v>1322.066024288431</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>16007.18922666661</v>
+        <v>89.60332073361897</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>-25937.38970212372</v>
+        <v>-724.9995078248512</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>25928.69095010845</v>
+        <v>998.7983469478718</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>-25018.74500419251</v>
+        <v>55.29819663671879</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>24023.25394606946</v>
+        <v>1991.154013478918</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>26520.78140720303</v>
+        <v>373.2664783476786</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>26517.35460750718</v>
+        <v>497.7412920205887</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>25180.97592026073</v>
+        <v>682.0034761809591</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>25194.59484550342</v>
+        <v>842.6744920986582</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>25378.63697633133</v>
+        <v>889.0510985489035</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>-24719.03961655198</v>
+        <v>-737.0235315822019</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>24769.19336045948</v>
+        <v>1049.550248749274</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>23185.86639144904</v>
+        <v>2144.529928183154</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>22736.1920838652</v>
+        <v>2101.028959686615</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>-19350.87097208797</v>
+        <v>382.9601032819955</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>18148.31941416716</v>
+        <v>-7.665729946763066</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>-103.8635216048247</v>
+        <v>276.1011288219963</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>-6858.611799515434</v>
+        <v>1224.551581189287</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>7483.9028014796</v>
+        <v>-923.1886243266292</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>-5904.245790899193</v>
+        <v>1365.364194156063</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>6287.809816693033</v>
+        <v>-1203.077514617241</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>5953.796701358174</v>
+        <v>-780.9145263567166</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>4753.752830365494</v>
+        <v>-2588.865176355377</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>554.7567740000271</v>
+        <v>897.176705038657</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>-1168.560893017614</v>
+        <v>371.6000474615932</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>-113.0097905589423</v>
+        <v>543.6174823463284</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>1395.631209205972</v>
+        <v>644.6558382718906</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>10694.18381754691</v>
+        <v>96.39545887199904</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>9219.450970747577</v>
+        <v>1860.613455057415</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>-8795.272873537977</v>
+        <v>486.9169262737444</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>-10382.35859337972</v>
+        <v>272.2328613183626</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>-10906.77336512111</v>
+        <v>-228.7671018806048</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>-11197.71099393045</v>
+        <v>-515.5638166575483</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>12470.3294095804</v>
+        <v>649.1338213044382</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>12264.53306889895</v>
+        <v>581.9889202706304</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>-3198.931701368766</v>
+        <v>294.803901698303</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>-1552.118989058286</v>
+        <v>677.8803750089585</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>-10201.35955108894</v>
+        <v>-647.1039511810515</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>-8482.986435822026</v>
+        <v>-949.9915651313044</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>-9174.341773195645</v>
+        <v>-915.5355020710402</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>-8589.225915239318</v>
+        <v>-489.1339463509228</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>-10666.34500540953</v>
+        <v>-1109.81659529294</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>10503.68716478517</v>
+        <v>1488.48678287511</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>-10095.35819037231</v>
+        <v>-1537.491523227475</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>3626.314172628608</v>
+        <v>-1431.690149072248</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>3605.553329474729</v>
+        <v>-1541.411707226843</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>2485.373575427096</v>
+        <v>-2528.1959909392</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>-4456.327576274214</v>
+        <v>-71.69118126070423</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>-2519.813777405575</v>
+        <v>38.5930312973736</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>3138.158923690822</v>
+        <v>234.9319342523449</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>16590.03815446447</v>
+        <v>-231.8625891986976</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>202.4555355226677</v>
+        <v>621.6513724450193</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>-14645.71917203173</v>
+        <v>-528.907974279826</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>-14732.92846415812</v>
+        <v>-711.7903291967335</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>-14744.66188952318</v>
+        <v>-543.0175978687486</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>15500.53919227392</v>
+        <v>972.2836573718412</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>-16560.57206805468</v>
+        <v>-642.3191850030745</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>-3423.310428624887</v>
+        <v>779.9062946366462</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>3945.300211252328</v>
+        <v>-309.4532120445137</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>4488.371105355147</v>
+        <v>-274.5494354421371</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>3527.819049329094</v>
+        <v>162.3870722406809</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>614.6997379115376</v>
+        <v>92.64048949435518</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>818.0311772888298</v>
+        <v>163.6074842640005</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>1091.996200406758</v>
+        <v>345.3129852213695</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>-3885.140101760643</v>
+        <v>370.9165147429072</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
-        <v>-3547.379499610423</v>
+        <v>385.2674312979399</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
-        <v>-3274.929308752971</v>
+        <v>374.7549321638443</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
-        <v>-3496.692265139223</v>
+        <v>718.7576651852791</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
-        <v>-2992.954516680484</v>
+        <v>614.4738782039836</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
-        <v>-3167.721349415769</v>
+        <v>516.5243599348147</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
-        <v>-7637.797768179441</v>
+        <v>373.6034225352265</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
-        <v>-7768.593530182908</v>
+        <v>339.9051098651975</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
-        <v>-1494.805269195215</v>
+        <v>-1033.612191297618</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
-        <v>-5890.247006186628</v>
+        <v>-656.5243272564478</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
-        <v>-4757.241549200168</v>
+        <v>-32.69486080900631</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
-        <v>-3894.877824744544</v>
+        <v>88.01097983755976</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
-        <v>-9128.323471080384</v>
+        <v>168.5507125119166</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
-        <v>-6703.240013673208</v>
+        <v>-199.1320960580386</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
-        <v>9496.53817616338</v>
+        <v>-72.79876565465598</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <v>7331.328213300613</v>
+        <v>-329.531110881746</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
-        <v>-8194.953591643916</v>
+        <v>1207.617493606764</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
-        <v>-7338.855356418931</v>
+        <v>1069.59609909002</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
-        <v>-2031.420407505945</v>
+        <v>848.3629757749726</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
-        <v>-53.26916582018634</v>
+        <v>-56.57144686961616</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
-        <v>-429.719285109568</v>
+        <v>-243.1796128478878</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
-        <v>-58.38352038210314</v>
+        <v>-107.7216559477238</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
-        <v>-272.1764826261218</v>
+        <v>200.2836708948369</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
-        <v>-198.4644335005844</v>
+        <v>-55.43470247318428</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <v>1208.443664910113</v>
+        <v>182.6811849970582</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
-        <v>1240.947788735248</v>
+        <v>235.478763115918</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
-        <v>2180.33396579995</v>
+        <v>150.0018983565305</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
-        <v>-61.70875633524159</v>
+        <v>-84.65459623748681</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
-        <v>5482.222262406707</v>
+        <v>975.5744355064141</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
-        <v>-3025.163354244864</v>
+        <v>92.49016556836388</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
-        <v>-3354.630932299837</v>
+        <v>4.850316319099801</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
-        <v>3006.179521790479</v>
+        <v>122.3145820553346</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
-        <v>954.4427815390335</v>
+        <v>168.6988774098444</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
-        <v>1246.474839391833</v>
+        <v>188.5259842932484</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
-        <v>1641.161515890795</v>
+        <v>474.0241230798239</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
-        <v>-361.7493842712638</v>
+        <v>115.3246385588478</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
-        <v>97.23345351616844</v>
+        <v>120.6630192772909</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118">
-        <v>1233.503745657138</v>
+        <v>248.1118422906653</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119">
-        <v>1259.43683450534</v>
+        <v>318.3052757910221</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120">
-        <v>-16.04636767762987</v>
+        <v>-58.59690644341712</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
-        <v>1421.733008271862</v>
+        <v>523.0012438827301</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
-        <v>1231.495343092422</v>
+        <v>330.9977539097773</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
-        <v>1540.54469883611</v>
+        <v>572.1773408911495</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
-        <v>1579.952708699796</v>
+        <v>700.5744745706005</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125">
-        <v>1502.49673860405</v>
+        <v>661.1209354430642</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
-        <v>-60805.45600652086</v>
+        <v>76.10176589337345</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127">
-        <v>-62060.26451284286</v>
+        <v>110.0740964383404</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
-        <v>-61052.8926601655</v>
+        <v>-43.46195803835833</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129">
-        <v>-60406.3731251725</v>
+        <v>488.7445506472644</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130">
-        <v>-63174.42664611954</v>
+        <v>344.5717599131317</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
-        <v>63672.06249381856</v>
+        <v>-117.1636295488436</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132">
-        <v>-51907.53366599275</v>
+        <v>-113.0726895469792</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
-        <v>-53692.94350098039</v>
+        <v>-612.4831212456547</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134">
-        <v>-53257.87876056931</v>
+        <v>-257.0655932874671</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
-        <v>-51091.56722250313</v>
+        <v>-177.8365246494876</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136">
-        <v>-50899.8619671645</v>
+        <v>-119.5366480131302</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137">
-        <v>-50948.12569560677</v>
+        <v>-64.34129900144909</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138">
-        <v>-51928.70446837266</v>
+        <v>-31.72544417815319</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
-        <v>-54175.88200893237</v>
+        <v>-196.9461136920934</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
-        <v>-53736.45180830042</v>
+        <v>-178.5961607362714</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141">
-        <v>-54984.63008656706</v>
+        <v>378.1663915040198</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
-        <v>-55277.2690914494</v>
+        <v>106.1201142904728</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
-        <v>-48700.82668825822</v>
+        <v>-418.0005815208447</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
-        <v>-50075.39791504665</v>
+        <v>-623.4127584899388</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
-        <v>-50877.71448602031</v>
+        <v>-518.0239044742491</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
-        <v>-46097.80184570808</v>
+        <v>-716.1109941063531</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
-        <v>-46964.62510964565</v>
+        <v>-846.714313047833</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148">
-        <v>-45089.00766983237</v>
+        <v>-824.5111321409267</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
-        <v>-44947.61134674039</v>
+        <v>-771.13724517557</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
-        <v>-39988.45623634795</v>
+        <v>-301.0465764620334</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151">
-        <v>42766.00150137037</v>
+        <v>468.846771181352</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
-        <v>403.1072679836582</v>
+        <v>69.48138611361372</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
-        <v>-396.153785032202</v>
+        <v>170.5378886486746</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
-        <v>-60676.94449802825</v>
+        <v>-757.4518091563973</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
-        <v>-60715.63406119579</v>
+        <v>-829.9612865186529</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
-        <v>-64317.15279889073</v>
+        <v>-780.2064149875679</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
-        <v>-64792.45293658922</v>
+        <v>-995.1671801309998</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158">
-        <v>-65317.88703375412</v>
+        <v>-149.6802584778402</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159">
-        <v>-65747.59344966632</v>
+        <v>-568.9665160942162</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160">
-        <v>921.639977696396</v>
+        <v>-358.1665095281391</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
-        <v>389.0358109230201</v>
+        <v>-518.7522310487369</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162">
-        <v>-511.102804841316</v>
+        <v>-751.702040069458</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163">
-        <v>-110.3020538907348</v>
+        <v>-445.8438367757167</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
-        <v>-520.5502852573978</v>
+        <v>-646.2084019185061</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165">
-        <v>-255.0277303742537</v>
+        <v>-549.3731121524198</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166">
-        <v>-910.2481979302692</v>
+        <v>-419.5784350539609</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
-        <v>-895.7861042303273</v>
+        <v>-494.529784128299</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168">
-        <v>-543.3257564952908</v>
+        <v>-339.3443298973527</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169">
-        <v>-622.9014101912275</v>
+        <v>-254.7789038923873</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
-        <v>-60895.47847105091</v>
+        <v>-601.3142031357993</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171">
-        <v>-58351.50359100624</v>
+        <v>-479.2683072987292</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
-        <v>-58121.76070662417</v>
+        <v>-472.2549634695877</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
-        <v>-63185.22709826731</v>
+        <v>-497.8179893945792</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
-        <v>-63075.41906224677</v>
+        <v>-233.6837690673404</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
-        <v>-63046.56977817711</v>
+        <v>-197.1451115503566</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
-        <v>3634.338246249179</v>
+        <v>60.43826643060896</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
-        <v>3296.985042464272</v>
+        <v>100.6804504917654</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178">
-        <v>3342.447813566642</v>
+        <v>151.7556221195771</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179">
-        <v>3242.603745990358</v>
+        <v>75.77171169397526</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180">
-        <v>3471.798244259083</v>
+        <v>220.6388013278092</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181">
-        <v>1287.93207996687</v>
+        <v>58.08182637302828</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
-        <v>3648.80205561165</v>
+        <v>581.5281282540867</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
-        <v>-54703.36284469137</v>
+        <v>639.6659889662729</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184">
-        <v>-72223.12679813978</v>
+        <v>-91.07481961229109</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
-        <v>69371.30443903081</v>
+        <v>254.5099800638703</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186">
-        <v>-73876.94210572295</v>
+        <v>896.3584048285204</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
-        <v>-73373.90451060863</v>
+        <v>989.19660834627</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
-        <v>-73849.6963704665</v>
+        <v>520.2201527114578</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
-        <v>-80450.2260066749</v>
+        <v>397.8895894449599</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190">
-        <v>-80925.66004764361</v>
+        <v>367.0486190814532</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
-        <v>-80831.49905943872</v>
+        <v>428.5230897468647</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192">
-        <v>5458.598092954115</v>
+        <v>711.825924844066</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
-        <v>5560.93314563788</v>
+        <v>820.9515961276214</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
-        <v>5494.6570561133</v>
+        <v>781.5643665946634</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195">
-        <v>-49058.99560961656</v>
+        <v>1357.040107415121</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196">
-        <v>-49456.18754358679</v>
+        <v>1725.141314925012</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197">
-        <v>59400.34768087484</v>
+        <v>-1951.79448092534</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
-        <v>3615.367518953476</v>
+        <v>-67.04297713258234</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199">
-        <v>-1195.696761240588</v>
+        <v>807.270846482221</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200">
-        <v>3242.772031036525</v>
+        <v>-394.8614470227326</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
-        <v>3195.256612730814</v>
+        <v>-199.8545711261784</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
-        <v>2867.927671192437</v>
+        <v>-442.131243518556</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
-        <v>1894.523705766278</v>
+        <v>-706.9077705204746</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
-        <v>1807.214615861551</v>
+        <v>-328.2557013933277</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
-        <v>3006.607757336752</v>
+        <v>-142.9777950001298</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
-        <v>3748.986642046582</v>
+        <v>-294.2557949984668</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
-        <v>2910.110127021846</v>
+        <v>-467.8115428519493</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
-        <v>3111.018121283609</v>
+        <v>-295.6164261356607</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
-        <v>3679.291764280094</v>
+        <v>-275.7766534647608</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210">
-        <v>2958.797290633112</v>
+        <v>-172.8961703729555</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
-        <v>2865.32728423134</v>
+        <v>-252.1720041476468</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212">
-        <v>-77320.62163005034</v>
+        <v>81.74568147718665</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
-        <v>-62767.95693794269</v>
+        <v>-467.6741560251085</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214">
-        <v>-62856.29798933925</v>
+        <v>-632.8378093556809</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215">
-        <v>-62523.50516807375</v>
+        <v>-466.0614566686327</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
-        <v>-62727.19224887715</v>
+        <v>-540.3792845208465</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
-        <v>-62959.06511913069</v>
+        <v>-598.4495240505493</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218">
-        <v>5867.138747758211</v>
+        <v>250.4988471220598</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219">
-        <v>3317.677219075654</v>
+        <v>-162.2693903830125</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220">
-        <v>2105.444056993915</v>
+        <v>-336.9875848909543</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
-        <v>450.2181948548036</v>
+        <v>-428.6412416076184</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <v>1082.009922850655</v>
+        <v>-484.5706142844476</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <v>2252.987537195151</v>
+        <v>-78.07620789549213</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224">
-        <v>2173.694225250227</v>
+        <v>48.5212071288552</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225">
-        <v>2110.132311397542</v>
+        <v>-53.55438556174489</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226">
-        <v>3676.368786729018</v>
+        <v>-173.8067370434722</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227">
-        <v>3585.201993948066</v>
+        <v>-188.698535434674</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
-        <v>2871.108678502259</v>
+        <v>-245.7006008778686</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229">
-        <v>3424.465305647711</v>
+        <v>153.5271354450958</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230">
-        <v>408.5284890715231</v>
+        <v>-305.2740095401299</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
-        <v>2185.143023333315</v>
+        <v>51.22855216872587</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232">
-        <v>2047.252031341452</v>
+        <v>114.2456264729907</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233">
-        <v>2973.368952204579</v>
+        <v>284.1094522179517</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234">
-        <v>3412.353359968442</v>
+        <v>-121.3987913532311</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235">
-        <v>31032.79848658621</v>
+        <v>-227.3175155646977</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
-        <v>30893.40515459322</v>
+        <v>-197.7994016274283</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237">
-        <v>28439.94028596287</v>
+        <v>-112.8512157043722</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
-        <v>29197.4047581399</v>
+        <v>-317.2427941174733</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
-        <v>29035.97190310188</v>
+        <v>-271.1910516416937</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
-        <v>29155.84321746047</v>
+        <v>-214.0019706283401</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
-        <v>26511.34316295659</v>
+        <v>-254.2577432281027</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242">
-        <v>17358.24985896407</v>
+        <v>-47.23145061339491</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243">
-        <v>-1021.494207331274</v>
+        <v>-107.4583336124402</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244">
-        <v>30259.83719080457</v>
+        <v>-252.4206228623638</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245">
-        <v>27363.18849675852</v>
+        <v>-199.5132739959399</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246">
-        <v>27789.01999422626</v>
+        <v>-102.6407576895163</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247">
-        <v>25086.49565815126</v>
+        <v>-158.4476256020587</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248">
-        <v>24878.49105409051</v>
+        <v>22.72197719991837</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249">
-        <v>-953.3599839892365</v>
+        <v>-12.28445328837198</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250">
-        <v>28098.80146135837</v>
+        <v>-132.9047839125476</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
-        <v>28851.87971246705</v>
+        <v>15.55497259985355</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
-        <v>27362.0090511862</v>
+        <v>450.454049301511</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253">
-        <v>2801.407548157481</v>
+        <v>299.2335163047049</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254">
-        <v>2451.115540787132</v>
+        <v>213.5723495453878</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
-        <v>32602.4606074973</v>
+        <v>682.8287944236922</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
-        <v>20927.61143276509</v>
+        <v>895.2474139456798</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257">
-        <v>-1685.40806651809</v>
+        <v>866.791243416873</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258">
-        <v>-1036.247669879524</v>
+        <v>890.4259621953976</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259">
-        <v>-528.0076333882103</v>
+        <v>907.0731723346942</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260">
-        <v>173.4839256136722</v>
+        <v>941.1396829037335</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261">
-        <v>7423.361609825116</v>
+        <v>924.4200346453431</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
-        <v>1131.428524583207</v>
+        <v>876.7540484325783</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263">
-        <v>322.4370029316153</v>
+        <v>1216.994143156704</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264">
-        <v>129.4821055735591</v>
+        <v>1206.769707132568</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265">
-        <v>4515.937721955638</v>
+        <v>1124.992367466901</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
-        <v>4562.857583015804</v>
+        <v>1165.85748835337</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
-        <v>6570.269934812061</v>
+        <v>1249.12960255309</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268">
-        <v>6492.060009332882</v>
+        <v>1133.567720716985</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269">
-        <v>842.6259688637238</v>
+        <v>783.9508865653161</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270">
-        <v>33548.73434231399</v>
+        <v>1109.621854707874</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271">
-        <v>31197.7868340044</v>
+        <v>903.0175782435548</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272">
-        <v>-1657.026416520848</v>
+        <v>1150.774295345694</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273">
-        <v>-1925.01685234803</v>
+        <v>1145.471219050125</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274">
-        <v>-1593.508726672713</v>
+        <v>1102.126409172454</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275">
-        <v>-1340.647044382169</v>
+        <v>1177.217807094282</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276">
-        <v>-906.7617285593037</v>
+        <v>1194.348553891006</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277">
-        <v>-426.1702139664978</v>
+        <v>1196.756692160164</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278">
-        <v>-424.9853194994653</v>
+        <v>1209.618765178132</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279">
-        <v>218.7563984829737</v>
+        <v>1222.353594355591</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
-        <v>4278.969574996601</v>
+        <v>1119.818766623243</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281">
-        <v>940.1060369288008</v>
+        <v>783.428813228212</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282">
-        <v>-23801.48318201219</v>
+        <v>1287.558556329204</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283">
-        <v>-24019.27296326749</v>
+        <v>1316.756310661816</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284">
-        <v>-25288.83611298444</v>
+        <v>3677.72142378441</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285">
-        <v>27971.67055480168</v>
+        <v>-1636.835893848684</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286">
-        <v>26476.01584097429</v>
+        <v>-145.284936637339</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287">
-        <v>-23134.59830926514</v>
+        <v>2097.870467267212</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288">
-        <v>-44182.62490387444</v>
+        <v>1680.839443016031</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289">
-        <v>-44614.88554327848</v>
+        <v>2417.474229851884</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290">
-        <v>-44005.25160959183</v>
+        <v>2575.007140426181</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291">
-        <v>46195.50729895832</v>
+        <v>2511.440885971757</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292">
-        <v>40587.29721514264</v>
+        <v>-2488.378050969757</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293">
-        <v>745.5521052788687</v>
+        <v>-107.4639965564955</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294">
-        <v>694.1623105411554</v>
+        <v>-61.67034331164405</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295">
-        <v>461.91505786741</v>
+        <v>16.8655372713868</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296">
-        <v>440.0212253041752</v>
+        <v>-20.726294094736</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297">
-        <v>-911.1154032824097</v>
+        <v>105.3086498606349</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298">
-        <v>-1221.399095763171</v>
+        <v>108.8238310832087</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299">
-        <v>-1430.352492281837</v>
+        <v>-177.2969717443899</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300">
-        <v>404.0475535680217</v>
+        <v>-125.9737552158659</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301">
-        <v>444.2559983382791</v>
+        <v>-127.7300307797959</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302">
-        <v>616.0801916084538</v>
+        <v>-295.5072670506034</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303">
-        <v>2308.411578639195</v>
+        <v>248.5428641532371</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304">
-        <v>31200.50563739586</v>
+        <v>1388.295244682487</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305">
-        <v>371.8214137252124</v>
+        <v>79.54429285466612</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306">
-        <v>1369.424766844208</v>
+        <v>316.7594714554131</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307">
-        <v>6949.520894363042</v>
+        <v>1394.311028608433</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308">
-        <v>43272.18371283742</v>
+        <v>1469.464586372527</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309">
-        <v>43161.73434580875</v>
+        <v>1504.609528260057</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310">
-        <v>44965.52626118184</v>
+        <v>1567.302058902228</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311">
-        <v>45817.30141370584</v>
+        <v>1262.183875247963</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312">
-        <v>44851.73448693314</v>
+        <v>1194.225201288833</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313">
-        <v>42794.07785211189</v>
+        <v>1396.165141432683</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314">
-        <v>39817.34372605288</v>
+        <v>1363.935189072103</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315">
-        <v>35974.94652376873</v>
+        <v>1307.938754299762</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316">
-        <v>6881.675629693498</v>
+        <v>1698.911458635128</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317">
-        <v>-32027.3291136604</v>
+        <v>913.8018386000359</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318">
-        <v>-30575.74995556257</v>
+        <v>943.9615195707929</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319">
-        <v>-33005.55744926292</v>
+        <v>850.2733834210532</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320">
-        <v>48159.87289508732</v>
+        <v>1988.527055289473</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321">
-        <v>42835.44315461927</v>
+        <v>844.5178435304272</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322">
-        <v>42320.68697508901</v>
+        <v>1114.631669486861</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323">
-        <v>42715.67858260446</v>
+        <v>1199.934604562402</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324">
-        <v>43644.25792138996</v>
+        <v>1471.211067272756</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325">
-        <v>43545.06978707716</v>
+        <v>1628.602057006965</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326">
-        <v>45457.37039442166</v>
+        <v>1482.563984570705</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327">
-        <v>45238.59378453386</v>
+        <v>1315.770911723579</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328">
-        <v>44143.19706578356</v>
+        <v>1097.494236920406</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329">
-        <v>44331.9258537639</v>
+        <v>1251.670885808771</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330">
-        <v>38083.28745413481</v>
+        <v>1649.504299737039</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331">
-        <v>35561.07490240392</v>
+        <v>1435.72293485102</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332">
-        <v>542.4019372208876</v>
+        <v>1748.772454490861</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333">
-        <v>19039.29534267216</v>
+        <v>257.5230180377651</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334">
-        <v>-16450.20450726449</v>
+        <v>-170.8028365027877</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335">
-        <v>-16715.36395861079</v>
+        <v>-281.9534096067132</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336">
-        <v>17717.40278719423</v>
+        <v>191.9831563138227</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337">
-        <v>-17292.36931432409</v>
+        <v>-45.50104826483612</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338">
-        <v>-16750.12630221334</v>
+        <v>-67.36808991704908</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339">
-        <v>-24512.72017573458</v>
+        <v>-357.93928945068</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340">
-        <v>-24314.57229718191</v>
+        <v>-307.4994597240988</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341">
-        <v>-23800.78856735655</v>
+        <v>-331.9588395292481</v>
       </c>
     </row>
   </sheetData>
@@ -2098,1152 +2098,1152 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>-446.7921331650156</v>
+        <v>-155.9716533801915</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>674.1350065442542</v>
+        <v>316.804155489149</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>31.38466307169678</v>
+        <v>59.36129116220692</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>48.00407969663507</v>
+        <v>-15.98497120086364</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>-5438.335967180993</v>
+        <v>-684.9126760444069</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>-4426.403818486438</v>
+        <v>130.8206361122739</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-1838.851703803405</v>
+        <v>1930.608040618585</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>-2286.734001919662</v>
+        <v>1468.43726039193</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>-1771.005097214934</v>
+        <v>2280.367541560284</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>-1417.443554330769</v>
+        <v>2377.635579446038</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>-25.33584679402043</v>
+        <v>1223.534838161579</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>6961.598103989685</v>
+        <v>961.4328971849624</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>6578.352074450982</v>
+        <v>974.1550792058417</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>6995.933520205477</v>
+        <v>1064.030943163198</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>-6037.953211479909</v>
+        <v>-736.7246841526306</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>-6047.903916861592</v>
+        <v>-822.8818121108519</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>643.8085838061568</v>
+        <v>717.7934199945995</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>1410.607724016222</v>
+        <v>1060.965187826414</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>1331.549649612138</v>
+        <v>1367.209431660888</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>980.7562419398701</v>
+        <v>1032.882565303911</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>57.67806793261152</v>
+        <v>98.15599068901058</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>-81.37410554656269</v>
+        <v>3.543476513063692</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>-72.90112768848724</v>
+        <v>89.36169673571959</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>-334.4787784812466</v>
+        <v>-160.6952000343611</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>-2385.815048981724</v>
+        <v>126.3770324183461</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>-1094.751810206033</v>
+        <v>584.6076716092466</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>-1215.891065108554</v>
+        <v>435.2774234491512</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>-2031.633429978755</v>
+        <v>587.8699193968164</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>-2753.857986749549</v>
+        <v>-362.3582318826452</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>-2464.602744080427</v>
+        <v>-23.70326233199103</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>-3179.095514499279</v>
+        <v>-593.4246679124649</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>-3208.924759275429</v>
+        <v>-625.6799105979949</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>3818.95463315277</v>
+        <v>776.7587312315542</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>-682.3644303428772</v>
+        <v>571.7563312326226</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>1048.007402026373</v>
+        <v>-204.315396090426</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>301.4736435780032</v>
+        <v>-559.8766252767882</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>15.87358727291455</v>
+        <v>879.7353148719716</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>-2374.75283507066</v>
+        <v>706.3569473351374</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>-2301.335290231942</v>
+        <v>506.8687300070026</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>1514.628366357856</v>
+        <v>366.4927808326227</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>-3509.615267882419</v>
+        <v>426.116707504332</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>-4246.6608449012</v>
+        <v>164.3588221142213</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>4062.382537269304</v>
+        <v>-270.9509160051385</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>-343.3450547120176</v>
+        <v>-313.5268071488562</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>-667.7824528916568</v>
+        <v>264.3059770772796</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>-663.3653815341466</v>
+        <v>302.4044077407001</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>-649.8395315011569</v>
+        <v>268.9064138433297</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>-799.0032335058604</v>
+        <v>428.0542703365442</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>1006.929968586527</v>
+        <v>-301.0900941941679</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>-913.8397640275774</v>
+        <v>326.5839562830366</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>1065.368749834856</v>
+        <v>-245.7643727536564</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>923.810366014269</v>
+        <v>27.11271967553812</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>-1246.058440158046</v>
+        <v>614.8597987322244</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>-1261.709279975353</v>
+        <v>683.2396421265958</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>2546.598932051464</v>
+        <v>892.82194850453</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>-2317.462042745088</v>
+        <v>-736.3989524592533</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>-2143.411698737942</v>
+        <v>-472.1832674422969</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>-3429.828449636034</v>
+        <v>-405.7245511723614</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>-1617.187346914733</v>
+        <v>134.9594911752074</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>-1707.801346676168</v>
+        <v>2.682793440352079</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>-1592.295976223539</v>
+        <v>253.5340333558685</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>-1517.377147797747</v>
+        <v>328.2205731174886</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>3097.537123626395</v>
+        <v>-115.9736653699038</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>-1822.398462232963</v>
+        <v>-266.7226623391598</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>-628.1892138472194</v>
+        <v>427.62988517134</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>-851.5163208941522</v>
+        <v>157.7262574692386</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>-684.9782042587553</v>
+        <v>334.6854208451796</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>-689.2641543390037</v>
+        <v>773.8889909156014</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>-1658.647719987267</v>
+        <v>-432.6186118653186</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>-2297.157185773041</v>
+        <v>-449.8028396860273</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>-2066.42560570254</v>
+        <v>426.64991520581</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>2345.260383719991</v>
+        <v>-146.1423641061974</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>1917.32729342618</v>
+        <v>-64.18432648078442</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>1672.909428155504</v>
+        <v>-809.383310909187</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>-1136.072876864427</v>
+        <v>1142.240669529272</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>-1034.410244858191</v>
+        <v>1440.135619386255</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>-481.9875865052568</v>
+        <v>-261.3278304291375</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>-2271.061481152582</v>
+        <v>1387.382219174359</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>-464.44142784004</v>
+        <v>-178.9295554450537</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>3241.991568006513</v>
+        <v>-542.7104747094545</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
-        <v>3250.64865883198</v>
+        <v>-532.0110179761577</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
-        <v>1257.778480236882</v>
+        <v>-623.7330503556959</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
-        <v>1247.032177549445</v>
+        <v>-642.7088876881135</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
-        <v>1583.892424463653</v>
+        <v>-630.08319991605</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
-        <v>1485.770858469354</v>
+        <v>-735.3630382283663</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
-        <v>839.7753104772164</v>
+        <v>-842.8891075747952</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
-        <v>820.1419190425404</v>
+        <v>-646.3449851343321</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
-        <v>110.9020841258243</v>
+        <v>-1351.558060047019</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
-        <v>-1852.649942392972</v>
+        <v>-950.8344425187406</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
-        <v>1697.321580925432</v>
+        <v>-279.5481169867544</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
-        <v>1649.545579173511</v>
+        <v>-388.2949503734799</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
-        <v>412.5118345637984</v>
+        <v>-460.8028201478919</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
-        <v>-4.684731537236132</v>
+        <v>24.15786166210705</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
-        <v>-257.1692623120076</v>
+        <v>-191.285518133947</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <v>-66.36540227425337</v>
+        <v>-31.3206509475222</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
-        <v>315.2510315485187</v>
+        <v>115.8946414287049</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
-        <v>-3.033055322392245</v>
+        <v>55.27302713400498</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
-        <v>-99.98906757299811</v>
+        <v>-10.65640983821207</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
-        <v>63.81542325215922</v>
+        <v>126.7137950296369</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
-        <v>-2502.576598087498</v>
+        <v>-26.52348426144751</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
-        <v>-2347.46150611448</v>
+        <v>97.28099095439165</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
-        <v>-2190.662266716649</v>
+        <v>120.7260880284895</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
-        <v>-2122.571467446047</v>
+        <v>276.5899505404508</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <v>165.3537417434565</v>
+        <v>132.2981625078806</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
-        <v>536.6631939356905</v>
+        <v>308.3786616814328</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
-        <v>841.0290991697514</v>
+        <v>292.0038133063976</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
-        <v>59.05299585410739</v>
+        <v>140.0871954401449</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
-        <v>-15390.39434164582</v>
+        <v>-95.5100618263581</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
-        <v>-15039.32016116627</v>
+        <v>134.7068573752684</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
-        <v>-14451.36515253874</v>
+        <v>172.4154172156686</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
-        <v>-15196.85714380926</v>
+        <v>-172.2771783716254</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
-        <v>-15653.67886159812</v>
+        <v>-361.1807509612462</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
-        <v>-90.82417923590172</v>
+        <v>-71.35363281452159</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
-        <v>80.49396510487701</v>
+        <v>-74.71352164071978</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116">
-        <v>-63.97900369352465</v>
+        <v>-120.5345500411319</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117">
-        <v>113.7110648321083</v>
+        <v>-32.47221117859028</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118">
-        <v>42.05400911135023</v>
+        <v>-25.76004818917155</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119">
-        <v>-45.04768173559683</v>
+        <v>22.295733127213</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120">
-        <v>-84.1749137595548</v>
+        <v>34.30580212035841</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
-        <v>434.759920909467</v>
+        <v>-355.6676104471539</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122">
-        <v>-444.605627398361</v>
+        <v>-526.2278849854915</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123">
-        <v>-557.7581565431009</v>
+        <v>-610.0333957041613</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124">
-        <v>-551.7448394540805</v>
+        <v>-706.3190488132411</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125">
-        <v>13183.82816898718</v>
+        <v>665.8337651667821</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126">
-        <v>11347.37636577449</v>
+        <v>-304.2060011340186</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127">
-        <v>11370.51968960688</v>
+        <v>-283.4054807679713</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
-        <v>-16113.75257767358</v>
+        <v>35.48446845235266</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129">
-        <v>15841.99405622133</v>
+        <v>173.850885717482</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130">
-        <v>-15137.25954689809</v>
+        <v>838.9155999191732</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131">
-        <v>-15026.91467127534</v>
+        <v>822.4809934826685</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132">
-        <v>614.5462947644073</v>
+        <v>-276.7247348688192</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133">
-        <v>553.124998888621</v>
+        <v>-285.1131509852165</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134">
-        <v>537.6842919736739</v>
+        <v>-169.9522974498082</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135">
-        <v>985.2486920389756</v>
+        <v>-105.7005410711486</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136">
-        <v>890.1426702217112</v>
+        <v>-129.8354543928564</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137">
-        <v>850.5676283392471</v>
+        <v>-116.1188233098269</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138">
-        <v>722.0385955998668</v>
+        <v>-35.927885965842</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139">
-        <v>-17050.28945617439</v>
+        <v>-1488.648704805894</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
-        <v>-16398.29006526284</v>
+        <v>-1029.195212060178</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141">
-        <v>702.7023859046324</v>
+        <v>-491.6835374198574</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
-        <v>188.8588568637634</v>
+        <v>-682.0463535315753</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
-        <v>362.149219478249</v>
+        <v>-447.4720428287321</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144">
-        <v>445.268906808538</v>
+        <v>-401.8921973937979</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145">
-        <v>373.1869051483366</v>
+        <v>-358.6539737521297</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146">
-        <v>414.1559501048749</v>
+        <v>-295.0937707877927</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147">
-        <v>1024.658002463899</v>
+        <v>-287.9585085808971</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148">
-        <v>872.8772985758783</v>
+        <v>-419.179137248609</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
-        <v>888.8407788846505</v>
+        <v>-392.5712356602095</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150">
-        <v>731.6715105397409</v>
+        <v>-380.2131808954196</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151">
-        <v>888.2606563379496</v>
+        <v>-341.8863715867558</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
-        <v>840.3401977248391</v>
+        <v>-372.8772853939203</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153">
-        <v>624.9011683369097</v>
+        <v>-261.0935892710616</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
-        <v>644.1579743514778</v>
+        <v>-127.0022101486752</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
-        <v>692.9564167199342</v>
+        <v>-62.44493879923333</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156">
-        <v>1370.45814783133</v>
+        <v>20.62328022564123</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
-        <v>1033.704131165426</v>
+        <v>-295.6125978644586</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158">
-        <v>798.2380530698134</v>
+        <v>-350.702983230292</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159">
-        <v>750.2372887168519</v>
+        <v>-411.91706344533</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160">
-        <v>17966.91687536884</v>
+        <v>1128.489641265836</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161">
-        <v>-16274.78254014211</v>
+        <v>-829.5891842241792</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162">
-        <v>-16967.05907836029</v>
+        <v>-304.1368756456202</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163">
-        <v>-16781.83276989167</v>
+        <v>-247.0407052941624</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
-        <v>532.388927876897</v>
+        <v>-466.4491096110773</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165">
-        <v>769.6870269192341</v>
+        <v>-182.0426749773089</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166">
-        <v>1466.3565432875</v>
+        <v>65.25689377159641</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167">
-        <v>1144.07246554405</v>
+        <v>-236.5041199445015</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168">
-        <v>-10905.80884827535</v>
+        <v>353.3553453425752</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169">
-        <v>8081.525661442985</v>
+        <v>-312.2632445991318</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170">
-        <v>8058.613488966603</v>
+        <v>-284.1165117622405</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171">
-        <v>8212.79271134058</v>
+        <v>-164.0913097759065</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
-        <v>8057.958760567244</v>
+        <v>-359.5014763309329</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
-        <v>8133.715313606991</v>
+        <v>-318.0914233708016</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
-        <v>8181.331865241882</v>
+        <v>-272.4098299848122</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
-        <v>-8969.159011353999</v>
+        <v>606.6767468964886</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
-        <v>8451.170832503247</v>
+        <v>-137.9968817730007</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177">
-        <v>8498.661853865311</v>
+        <v>-92.51128840018491</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178">
-        <v>8417.400089099683</v>
+        <v>-47.17930827935882</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179">
-        <v>9176.650388228263</v>
+        <v>647.7251085875758</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180">
-        <v>8644.279037067592</v>
+        <v>704.2241348212215</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181">
-        <v>711.2322233032537</v>
+        <v>836.4698697594041</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182">
-        <v>1269.879015245019</v>
+        <v>867.9968407774611</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183">
-        <v>4269.208732992021</v>
+        <v>-1193.840918121556</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184">
-        <v>4294.115827948426</v>
+        <v>-1203.908257665335</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185">
-        <v>4630.589182400159</v>
+        <v>-872.5485524988217</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186">
-        <v>4378.858566295108</v>
+        <v>-716.3848615564584</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
-        <v>3975.001193330538</v>
+        <v>-650.2049288846802</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
-        <v>3844.119096480947</v>
+        <v>-664.2606972441999</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
-        <v>3696.822897513401</v>
+        <v>-1409.578606623631</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190">
-        <v>2627.220193146817</v>
+        <v>-2020.465622208352</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191">
-        <v>-7680.896541563665</v>
+        <v>1579.268467291663</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192">
-        <v>7234.287069508102</v>
+        <v>-1536.579933445604</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
-        <v>-6359.186085863698</v>
+        <v>1303.618099213312</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
-        <v>-5701.720597898799</v>
+        <v>1773.796276009549</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195">
-        <v>-5650.989438577915</v>
+        <v>1685.464589856051</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196">
-        <v>-4836.430933921918</v>
+        <v>1337.398432399597</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197">
-        <v>11524.00512745783</v>
+        <v>1781.522683758111</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198">
-        <v>11433.44770142349</v>
+        <v>1410.08357507517</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199">
-        <v>2113.777432681525</v>
+        <v>766.5119560497506</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200">
-        <v>2202.089990180386</v>
+        <v>-2464.121598701417</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201">
-        <v>361.591679519976</v>
+        <v>65.23227551280428</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
-        <v>-209.808426564139</v>
+        <v>66.2320148247757</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
-        <v>-258.8052617467645</v>
+        <v>-31.09150000162277</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204">
-        <v>-234.6511676361942</v>
+        <v>-37.83905631307456</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205">
-        <v>382.3243929939034</v>
+        <v>163.6066620441055</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
-        <v>230.9659990339024</v>
+        <v>-87.60754064067009</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
-        <v>319.7117390570044</v>
+        <v>-7.706267477877158</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208">
-        <v>-97.65445149970654</v>
+        <v>213.0631445569742</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209">
-        <v>321.9401670376308</v>
+        <v>-67.56769763460737</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210">
-        <v>-15.70182175134904</v>
+        <v>-263.6726943504501</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211">
-        <v>52.56862247030742</v>
+        <v>284.6237542425838</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212">
-        <v>1163.253726960111</v>
+        <v>614.4415022912683</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213">
-        <v>1518.017491998433</v>
+        <v>419.435902613533</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214">
-        <v>2815.522028372557</v>
+        <v>1341.036567902796</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215">
-        <v>2782.841778514142</v>
+        <v>1307.233921393821</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
-        <v>3348.549475729858</v>
+        <v>1357.472420867636</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
-        <v>11235.78618177056</v>
+        <v>1427.741269882967</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218">
-        <v>11121.94905213408</v>
+        <v>1458.515782401076</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219">
-        <v>10266.45028683328</v>
+        <v>1443.18982673391</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220">
-        <v>1903.137610703635</v>
+        <v>1511.742633660552</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221">
-        <v>1843.257555421068</v>
+        <v>1498.719854344495</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <v>471.9048079435444</v>
+        <v>189.5581471292882</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <v>-5331.194827536196</v>
+        <v>974.799087344236</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224">
-        <v>-4910.379643359619</v>
+        <v>1037.548028176686</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225">
-        <v>4837.021167349404</v>
+        <v>187.3011248792616</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226">
-        <v>4905.745130582453</v>
+        <v>182.477633612066</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227">
-        <v>4926.636210886103</v>
+        <v>172.1410323514065</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228">
-        <v>-5135.124613103801</v>
+        <v>-248.5097877100411</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229">
-        <v>-4886.978844385989</v>
+        <v>-297.0028979272719</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230">
-        <v>-3933.454290717635</v>
+        <v>749.5635023661077</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
-        <v>-3949.811373433931</v>
+        <v>773.3786676152351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>